<commit_message>
Deploying to gh-pages from @ OP-TED/OP-TED.github.io@2f9a1634ceabad52036c7d1c00eb861d36c71170 🚀
</commit_message>
<xml_diff>
--- a/ESPD-EDM/2.0.0/_attachments/dist/cl/xlsx/BACH-DataBase-Ratios.xlsx
+++ b/ESPD-EDM/2.0.0/_attachments/dist/cl/xlsx/BACH-DataBase-Ratios.xlsx
@@ -1,19 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Develop\ESPD\GitHub\ESPD-EDM\docs\src\main\asciidoc\dist\cl\xlsx\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="960" yWindow="330" windowWidth="17580" windowHeight="10230"/>
+    <workbookView xWindow="960" yWindow="324" windowWidth="17580" windowHeight="10236"/>
   </bookViews>
   <sheets>
     <sheet name="Ratios" sheetId="1" r:id="rId1"/>
   </sheets>
+  <externalReferences>
+    <externalReference r:id="rId2"/>
+  </externalReferences>
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">Ratios!$A$1:$H$108</definedName>
     <definedName name="Divisao" localSheetId="0">#REF!</definedName>
@@ -566,8 +564,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="20" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="20">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -818,6 +816,9 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
@@ -842,6 +843,12 @@
     <xf numFmtId="0" fontId="14" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -858,6 +865,15 @@
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="11"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -874,24 +890,6 @@
     </xf>
     <xf numFmtId="0" fontId="15" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -899,14 +897,6 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -960,6 +950,29 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Income Statement"/>
+      <sheetName val="BS - Assets"/>
+      <sheetName val="BS - Liabilities"/>
+      <sheetName val="Ratios"/>
+      <sheetName val="Notes"/>
+      <sheetName val="NACE"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0"/>
+      <sheetData sheetId="1"/>
+      <sheetData sheetId="2"/>
+      <sheetData sheetId="3"/>
+      <sheetData sheetId="4"/>
+      <sheetData sheetId="5"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
@@ -1003,7 +1016,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1035,10 +1048,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1070,7 +1082,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1246,1294 +1257,1212 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr>
     <tabColor rgb="FF9BBB59"/>
   </sheetPr>
   <dimension ref="B1:H106"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A68" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G25" sqref="G25"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="13.8"/>
   <cols>
-    <col min="1" max="1" width="2.42578125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="0.85546875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="6.85546875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="47.5703125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="2.44140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="0.88671875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="6.88671875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="47.5546875" style="1" customWidth="1"/>
     <col min="5" max="5" width="47" style="2" customWidth="1"/>
-    <col min="6" max="6" width="24.5703125" style="3" customWidth="1"/>
+    <col min="6" max="6" width="24.5546875" style="3" customWidth="1"/>
     <col min="7" max="7" width="31" style="4" customWidth="1"/>
-    <col min="8" max="8" width="2.28515625" style="1" customWidth="1"/>
-    <col min="9" max="16384" width="9.140625" style="1"/>
+    <col min="8" max="8" width="2.33203125" style="1" customWidth="1"/>
+    <col min="9" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:8" ht="7.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="2" spans="2:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="2:8" ht="7.5" customHeight="1"/>
+    <row r="2" spans="2:8" ht="12.75" customHeight="1">
       <c r="B2" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="30" t="s">
+      <c r="C2" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="30"/>
-      <c r="E2" s="30"/>
-      <c r="F2" s="30"/>
-      <c r="G2" s="30"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
       <c r="H2" s="5"/>
     </row>
-    <row r="3" spans="2:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:8" ht="12.75" customHeight="1">
       <c r="B3" s="5"/>
-      <c r="C3" s="30"/>
-      <c r="D3" s="30"/>
-      <c r="E3" s="30"/>
-      <c r="F3" s="30"/>
-      <c r="G3" s="30"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="6"/>
+      <c r="G3" s="6"/>
       <c r="H3" s="5"/>
     </row>
-    <row r="4" spans="2:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:8" ht="12.75" customHeight="1">
       <c r="B4" s="5"/>
-      <c r="C4" s="30"/>
-      <c r="D4" s="30"/>
-      <c r="E4" s="30"/>
-      <c r="F4" s="30"/>
-      <c r="G4" s="30"/>
+      <c r="C4" s="6"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="6"/>
+      <c r="G4" s="6"/>
       <c r="H4" s="5"/>
     </row>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="G5" s="6" t="s">
+    <row r="5" spans="2:8">
+      <c r="G5" s="7" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="G6" s="7" t="s">
+    <row r="6" spans="2:8">
+      <c r="G6" s="8" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="G7" s="8" t="s">
+    <row r="7" spans="2:8">
+      <c r="G7" s="9" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="G8" s="8" t="s">
+    <row r="8" spans="2:8">
+      <c r="G8" s="9" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="G9" s="9" t="s">
+    <row r="9" spans="2:8">
+      <c r="G9" s="10" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="2:8" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C10" s="10" t="s">
+    <row r="10" spans="2:8" ht="14.4" thickBot="1">
+      <c r="C10" s="11" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="2:8" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C11" s="11" t="s">
+    <row r="11" spans="2:8" ht="27.75" customHeight="1" thickBot="1">
+      <c r="C11" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="D11" s="12" t="s">
+      <c r="D11" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="E11" s="13" t="s">
+      <c r="E11" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="F11" s="28" t="s">
+      <c r="F11" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="G11" s="29"/>
-    </row>
-    <row r="12" spans="2:8" ht="3" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C12" s="14"/>
-      <c r="D12" s="15"/>
-      <c r="E12" s="16"/>
-      <c r="F12" s="17"/>
-      <c r="G12" s="18"/>
-    </row>
-    <row r="13" spans="2:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C13" s="25" t="s">
+      <c r="G11" s="16"/>
+    </row>
+    <row r="12" spans="2:8" ht="3" customHeight="1" thickBot="1">
+      <c r="C12" s="17"/>
+      <c r="D12" s="18"/>
+      <c r="E12" s="19"/>
+      <c r="F12" s="20"/>
+      <c r="G12" s="21"/>
+    </row>
+    <row r="13" spans="2:8" ht="15" customHeight="1" thickBot="1">
+      <c r="C13" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="D13" s="26" t="s">
+      <c r="D13" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="E13" s="27" t="s">
+      <c r="E13" s="24" t="s">
         <v>13</v>
       </c>
-      <c r="F13" s="19" t="s">
-        <v>14</v>
-      </c>
-      <c r="G13" s="20" t="s">
+      <c r="F13" s="25" t="s">
+        <v>14</v>
+      </c>
+      <c r="G13" s="26" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="2:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C14" s="25"/>
-      <c r="D14" s="26"/>
-      <c r="E14" s="27"/>
-      <c r="F14" s="19" t="s">
-        <v>16</v>
-      </c>
-      <c r="G14" s="20" t="s">
+    <row r="14" spans="2:8" ht="15" customHeight="1" thickBot="1">
+      <c r="C14" s="22"/>
+      <c r="D14" s="23"/>
+      <c r="E14" s="24"/>
+      <c r="F14" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="G14" s="26" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="15" spans="2:8" ht="3" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C15" s="14"/>
-      <c r="D15" s="15"/>
-      <c r="E15" s="16"/>
-      <c r="F15" s="17"/>
-      <c r="G15" s="18"/>
-    </row>
-    <row r="16" spans="2:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C16" s="25" t="s">
+    <row r="15" spans="2:8" ht="3" customHeight="1" thickBot="1">
+      <c r="C15" s="17"/>
+      <c r="D15" s="18"/>
+      <c r="E15" s="19"/>
+      <c r="F15" s="20"/>
+      <c r="G15" s="21"/>
+    </row>
+    <row r="16" spans="2:8" ht="15" customHeight="1" thickBot="1">
+      <c r="C16" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="D16" s="26" t="s">
+      <c r="D16" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="E16" s="27" t="s">
+      <c r="E16" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="F16" s="19" t="s">
-        <v>14</v>
-      </c>
-      <c r="G16" s="20" t="s">
+      <c r="F16" s="25" t="s">
+        <v>14</v>
+      </c>
+      <c r="G16" s="26" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="17" spans="3:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C17" s="25"/>
-      <c r="D17" s="26"/>
-      <c r="E17" s="27"/>
-      <c r="F17" s="19" t="s">
-        <v>16</v>
-      </c>
-      <c r="G17" s="20" t="s">
+    <row r="17" spans="3:7" ht="15" customHeight="1" thickBot="1">
+      <c r="C17" s="22"/>
+      <c r="D17" s="23"/>
+      <c r="E17" s="24"/>
+      <c r="F17" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="G17" s="26" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="18" spans="3:7" ht="3" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C18" s="14"/>
-      <c r="D18" s="15"/>
-      <c r="E18" s="16"/>
-      <c r="F18" s="17"/>
-      <c r="G18" s="18"/>
-    </row>
-    <row r="19" spans="3:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C19" s="25" t="s">
+    <row r="18" spans="3:7" ht="3" customHeight="1" thickBot="1">
+      <c r="C18" s="17"/>
+      <c r="D18" s="18"/>
+      <c r="E18" s="19"/>
+      <c r="F18" s="20"/>
+      <c r="G18" s="21"/>
+    </row>
+    <row r="19" spans="3:7" ht="15" customHeight="1" thickBot="1">
+      <c r="C19" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="D19" s="26" t="s">
+      <c r="D19" s="23" t="s">
         <v>23</v>
       </c>
-      <c r="E19" s="27" t="s">
+      <c r="E19" s="24" t="s">
         <v>24</v>
       </c>
-      <c r="F19" s="19" t="s">
-        <v>14</v>
-      </c>
-      <c r="G19" s="20" t="s">
+      <c r="F19" s="25" t="s">
+        <v>14</v>
+      </c>
+      <c r="G19" s="26" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="20" spans="3:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C20" s="25"/>
-      <c r="D20" s="26"/>
-      <c r="E20" s="27"/>
-      <c r="F20" s="19" t="s">
-        <v>16</v>
-      </c>
-      <c r="G20" s="20" t="s">
+    <row r="20" spans="3:7" ht="15" customHeight="1" thickBot="1">
+      <c r="C20" s="22"/>
+      <c r="D20" s="23"/>
+      <c r="E20" s="24"/>
+      <c r="F20" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="G20" s="26" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="21" spans="3:7" ht="3" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C21" s="14"/>
-      <c r="D21" s="15"/>
-      <c r="E21" s="16"/>
-      <c r="F21" s="17"/>
-      <c r="G21" s="18"/>
-    </row>
-    <row r="22" spans="3:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C22" s="25" t="s">
+    <row r="21" spans="3:7" ht="3" customHeight="1" thickBot="1">
+      <c r="C21" s="17"/>
+      <c r="D21" s="18"/>
+      <c r="E21" s="19"/>
+      <c r="F21" s="20"/>
+      <c r="G21" s="21"/>
+    </row>
+    <row r="22" spans="3:7" ht="15" customHeight="1" thickBot="1">
+      <c r="C22" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="D22" s="26" t="s">
+      <c r="D22" s="23" t="s">
         <v>27</v>
       </c>
-      <c r="E22" s="27" t="s">
+      <c r="E22" s="24" t="s">
         <v>28</v>
       </c>
-      <c r="F22" s="19" t="s">
-        <v>14</v>
-      </c>
-      <c r="G22" s="20" t="s">
+      <c r="F22" s="25" t="s">
+        <v>14</v>
+      </c>
+      <c r="G22" s="26" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="23" spans="3:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C23" s="25"/>
-      <c r="D23" s="26"/>
-      <c r="E23" s="27"/>
-      <c r="F23" s="19" t="s">
-        <v>16</v>
-      </c>
-      <c r="G23" s="20" t="s">
+    <row r="23" spans="3:7" ht="15" customHeight="1" thickBot="1">
+      <c r="C23" s="22"/>
+      <c r="D23" s="23"/>
+      <c r="E23" s="24"/>
+      <c r="F23" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="G23" s="26" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="24" spans="3:7" ht="3" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C24" s="14"/>
-      <c r="D24" s="15"/>
-      <c r="E24" s="16"/>
-      <c r="F24" s="17"/>
-      <c r="G24" s="18"/>
-    </row>
-    <row r="25" spans="3:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C25" s="25" t="s">
+    <row r="24" spans="3:7" ht="3" customHeight="1" thickBot="1">
+      <c r="C24" s="17"/>
+      <c r="D24" s="18"/>
+      <c r="E24" s="19"/>
+      <c r="F24" s="20"/>
+      <c r="G24" s="21"/>
+    </row>
+    <row r="25" spans="3:7" ht="15" customHeight="1" thickBot="1">
+      <c r="C25" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="D25" s="26" t="s">
+      <c r="D25" s="23" t="s">
         <v>31</v>
       </c>
-      <c r="E25" s="27" t="s">
+      <c r="E25" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="F25" s="19" t="s">
-        <v>14</v>
-      </c>
-      <c r="G25" s="20" t="s">
+      <c r="F25" s="25" t="s">
+        <v>14</v>
+      </c>
+      <c r="G25" s="26" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="26" spans="3:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C26" s="25"/>
-      <c r="D26" s="26"/>
-      <c r="E26" s="27"/>
-      <c r="F26" s="19" t="s">
-        <v>16</v>
-      </c>
-      <c r="G26" s="20" t="s">
+    <row r="26" spans="3:7" ht="15" customHeight="1" thickBot="1">
+      <c r="C26" s="22"/>
+      <c r="D26" s="23"/>
+      <c r="E26" s="24"/>
+      <c r="F26" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="G26" s="26" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="27" spans="3:7" ht="3" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C27" s="14"/>
-      <c r="D27" s="15"/>
-      <c r="E27" s="16"/>
-      <c r="F27" s="17"/>
-      <c r="G27" s="18"/>
-    </row>
-    <row r="28" spans="3:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C28" s="25" t="s">
+    <row r="27" spans="3:7" ht="3" customHeight="1" thickBot="1">
+      <c r="C27" s="17"/>
+      <c r="D27" s="18"/>
+      <c r="E27" s="19"/>
+      <c r="F27" s="20"/>
+      <c r="G27" s="21"/>
+    </row>
+    <row r="28" spans="3:7" ht="15" customHeight="1" thickBot="1">
+      <c r="C28" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="D28" s="26" t="s">
+      <c r="D28" s="23" t="s">
         <v>35</v>
       </c>
-      <c r="E28" s="27" t="s">
+      <c r="E28" s="24" t="s">
         <v>36</v>
       </c>
-      <c r="F28" s="19" t="s">
-        <v>14</v>
-      </c>
-      <c r="G28" s="20" t="s">
+      <c r="F28" s="25" t="s">
+        <v>14</v>
+      </c>
+      <c r="G28" s="26" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="29" spans="3:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C29" s="25"/>
-      <c r="D29" s="26"/>
-      <c r="E29" s="27"/>
-      <c r="F29" s="19" t="s">
-        <v>16</v>
-      </c>
-      <c r="G29" s="20" t="s">
+    <row r="29" spans="3:7" ht="15" customHeight="1" thickBot="1">
+      <c r="C29" s="22"/>
+      <c r="D29" s="23"/>
+      <c r="E29" s="24"/>
+      <c r="F29" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="G29" s="26" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="30" spans="3:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C30" s="21"/>
-      <c r="D30" s="22"/>
-      <c r="E30" s="22"/>
-      <c r="F30" s="23"/>
-      <c r="G30" s="24"/>
-    </row>
-    <row r="31" spans="3:7" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C31" s="11" t="s">
+    <row r="30" spans="3:7" ht="14.4" thickBot="1">
+      <c r="C30" s="27"/>
+      <c r="D30" s="28"/>
+      <c r="E30" s="28"/>
+      <c r="F30" s="29"/>
+      <c r="G30" s="30"/>
+    </row>
+    <row r="31" spans="3:7" ht="27.75" customHeight="1" thickBot="1">
+      <c r="C31" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="D31" s="12" t="s">
+      <c r="D31" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="E31" s="13" t="s">
+      <c r="E31" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="F31" s="28" t="s">
+      <c r="F31" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="G31" s="29"/>
-    </row>
-    <row r="32" spans="3:7" ht="3" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C32" s="14"/>
-      <c r="D32" s="15"/>
-      <c r="E32" s="16"/>
-      <c r="F32" s="17"/>
-      <c r="G32" s="18"/>
-    </row>
-    <row r="33" spans="3:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C33" s="25" t="s">
+      <c r="G31" s="16"/>
+    </row>
+    <row r="32" spans="3:7" ht="3" customHeight="1" thickBot="1">
+      <c r="C32" s="17"/>
+      <c r="D32" s="18"/>
+      <c r="E32" s="19"/>
+      <c r="F32" s="20"/>
+      <c r="G32" s="21"/>
+    </row>
+    <row r="33" spans="3:7" ht="15" customHeight="1" thickBot="1">
+      <c r="C33" s="22" t="s">
         <v>40</v>
       </c>
-      <c r="D33" s="26" t="s">
+      <c r="D33" s="23" t="s">
         <v>41</v>
       </c>
-      <c r="E33" s="27" t="s">
+      <c r="E33" s="24" t="s">
         <v>42</v>
       </c>
-      <c r="F33" s="19" t="s">
-        <v>14</v>
-      </c>
-      <c r="G33" s="20" t="s">
+      <c r="F33" s="25" t="s">
+        <v>14</v>
+      </c>
+      <c r="G33" s="26" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="34" spans="3:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C34" s="25"/>
-      <c r="D34" s="26"/>
-      <c r="E34" s="27"/>
-      <c r="F34" s="19" t="s">
-        <v>16</v>
-      </c>
-      <c r="G34" s="20" t="s">
+    <row r="34" spans="3:7" ht="15" customHeight="1" thickBot="1">
+      <c r="C34" s="22"/>
+      <c r="D34" s="23"/>
+      <c r="E34" s="24"/>
+      <c r="F34" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="G34" s="26" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="35" spans="3:7" ht="3" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C35" s="14"/>
-      <c r="D35" s="15"/>
-      <c r="E35" s="16"/>
-      <c r="F35" s="17"/>
-      <c r="G35" s="18"/>
-    </row>
-    <row r="36" spans="3:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C36" s="25" t="s">
+    <row r="35" spans="3:7" ht="3" customHeight="1" thickBot="1">
+      <c r="C35" s="17"/>
+      <c r="D35" s="18"/>
+      <c r="E35" s="19"/>
+      <c r="F35" s="20"/>
+      <c r="G35" s="21"/>
+    </row>
+    <row r="36" spans="3:7" ht="15" customHeight="1" thickBot="1">
+      <c r="C36" s="22" t="s">
         <v>45</v>
       </c>
-      <c r="D36" s="26" t="s">
+      <c r="D36" s="23" t="s">
         <v>46</v>
       </c>
-      <c r="E36" s="27" t="s">
+      <c r="E36" s="24" t="s">
         <v>47</v>
       </c>
-      <c r="F36" s="19" t="s">
-        <v>14</v>
-      </c>
-      <c r="G36" s="20" t="s">
+      <c r="F36" s="25" t="s">
+        <v>14</v>
+      </c>
+      <c r="G36" s="26" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="37" spans="3:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C37" s="25"/>
-      <c r="D37" s="26"/>
-      <c r="E37" s="27"/>
-      <c r="F37" s="19" t="s">
-        <v>16</v>
-      </c>
-      <c r="G37" s="20" t="s">
+    <row r="37" spans="3:7" ht="15" customHeight="1" thickBot="1">
+      <c r="C37" s="22"/>
+      <c r="D37" s="23"/>
+      <c r="E37" s="24"/>
+      <c r="F37" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="G37" s="26" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="38" spans="3:7" ht="3" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C38" s="14"/>
-      <c r="D38" s="15"/>
-      <c r="E38" s="16"/>
-      <c r="F38" s="17"/>
-      <c r="G38" s="18"/>
-    </row>
-    <row r="39" spans="3:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C39" s="25" t="s">
+    <row r="38" spans="3:7" ht="3" customHeight="1" thickBot="1">
+      <c r="C38" s="17"/>
+      <c r="D38" s="18"/>
+      <c r="E38" s="19"/>
+      <c r="F38" s="20"/>
+      <c r="G38" s="21"/>
+    </row>
+    <row r="39" spans="3:7" ht="15" customHeight="1" thickBot="1">
+      <c r="C39" s="22" t="s">
         <v>49</v>
       </c>
-      <c r="D39" s="26" t="s">
+      <c r="D39" s="23" t="s">
         <v>50</v>
       </c>
-      <c r="E39" s="27" t="s">
+      <c r="E39" s="24" t="s">
         <v>51</v>
       </c>
-      <c r="F39" s="19" t="s">
-        <v>14</v>
-      </c>
-      <c r="G39" s="20" t="s">
+      <c r="F39" s="25" t="s">
+        <v>14</v>
+      </c>
+      <c r="G39" s="26" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="40" spans="3:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C40" s="25"/>
-      <c r="D40" s="26"/>
-      <c r="E40" s="27"/>
-      <c r="F40" s="19" t="s">
-        <v>16</v>
-      </c>
-      <c r="G40" s="20" t="s">
+    <row r="40" spans="3:7" ht="15" customHeight="1" thickBot="1">
+      <c r="C40" s="22"/>
+      <c r="D40" s="23"/>
+      <c r="E40" s="24"/>
+      <c r="F40" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="G40" s="26" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="41" spans="3:7" ht="3" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C41" s="14"/>
-      <c r="D41" s="15"/>
-      <c r="E41" s="16"/>
-      <c r="F41" s="17"/>
-      <c r="G41" s="18"/>
-    </row>
-    <row r="42" spans="3:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C42" s="25" t="s">
+    <row r="41" spans="3:7" ht="3" customHeight="1" thickBot="1">
+      <c r="C41" s="17"/>
+      <c r="D41" s="18"/>
+      <c r="E41" s="19"/>
+      <c r="F41" s="20"/>
+      <c r="G41" s="21"/>
+    </row>
+    <row r="42" spans="3:7" ht="15" customHeight="1" thickBot="1">
+      <c r="C42" s="22" t="s">
         <v>54</v>
       </c>
-      <c r="D42" s="26" t="s">
+      <c r="D42" s="23" t="s">
         <v>55</v>
       </c>
-      <c r="E42" s="27" t="s">
+      <c r="E42" s="24" t="s">
         <v>55</v>
       </c>
-      <c r="F42" s="19" t="s">
-        <v>14</v>
-      </c>
-      <c r="G42" s="20" t="s">
+      <c r="F42" s="25" t="s">
+        <v>14</v>
+      </c>
+      <c r="G42" s="26" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="43" spans="3:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C43" s="25"/>
-      <c r="D43" s="26"/>
-      <c r="E43" s="27"/>
-      <c r="F43" s="19" t="s">
-        <v>16</v>
-      </c>
-      <c r="G43" s="20" t="s">
+    <row r="43" spans="3:7" ht="15" customHeight="1" thickBot="1">
+      <c r="C43" s="22"/>
+      <c r="D43" s="23"/>
+      <c r="E43" s="24"/>
+      <c r="F43" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="G43" s="26" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="44" spans="3:7" ht="3" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C44" s="14"/>
-      <c r="D44" s="15"/>
-      <c r="E44" s="16"/>
-      <c r="F44" s="17"/>
-      <c r="G44" s="18"/>
-    </row>
-    <row r="45" spans="3:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C45" s="25" t="s">
+    <row r="44" spans="3:7" ht="3" customHeight="1" thickBot="1">
+      <c r="C44" s="17"/>
+      <c r="D44" s="18"/>
+      <c r="E44" s="19"/>
+      <c r="F44" s="20"/>
+      <c r="G44" s="21"/>
+    </row>
+    <row r="45" spans="3:7" ht="15" customHeight="1" thickBot="1">
+      <c r="C45" s="22" t="s">
         <v>58</v>
       </c>
-      <c r="D45" s="26" t="s">
+      <c r="D45" s="23" t="s">
         <v>59</v>
       </c>
-      <c r="E45" s="27" t="s">
+      <c r="E45" s="24" t="s">
         <v>59</v>
       </c>
-      <c r="F45" s="19" t="s">
-        <v>14</v>
-      </c>
-      <c r="G45" s="20" t="s">
+      <c r="F45" s="25" t="s">
+        <v>14</v>
+      </c>
+      <c r="G45" s="26" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="46" spans="3:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C46" s="25"/>
-      <c r="D46" s="26"/>
-      <c r="E46" s="27"/>
-      <c r="F46" s="19" t="s">
-        <v>16</v>
-      </c>
-      <c r="G46" s="20" t="s">
+    <row r="46" spans="3:7" ht="15" customHeight="1" thickBot="1">
+      <c r="C46" s="22"/>
+      <c r="D46" s="23"/>
+      <c r="E46" s="24"/>
+      <c r="F46" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="G46" s="26" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="47" spans="3:7" ht="3" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C47" s="14"/>
-      <c r="D47" s="15"/>
-      <c r="E47" s="16"/>
-      <c r="F47" s="17"/>
-      <c r="G47" s="18"/>
-    </row>
-    <row r="48" spans="3:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C48" s="25" t="s">
+    <row r="47" spans="3:7" ht="3" customHeight="1" thickBot="1">
+      <c r="C47" s="17"/>
+      <c r="D47" s="18"/>
+      <c r="E47" s="19"/>
+      <c r="F47" s="20"/>
+      <c r="G47" s="21"/>
+    </row>
+    <row r="48" spans="3:7" ht="15" customHeight="1" thickBot="1">
+      <c r="C48" s="22" t="s">
         <v>61</v>
       </c>
-      <c r="D48" s="26" t="s">
+      <c r="D48" s="23" t="s">
         <v>62</v>
       </c>
-      <c r="E48" s="27" t="s">
+      <c r="E48" s="24" t="s">
         <v>63</v>
       </c>
-      <c r="F48" s="19" t="s">
-        <v>14</v>
-      </c>
-      <c r="G48" s="20" t="s">
+      <c r="F48" s="25" t="s">
+        <v>14</v>
+      </c>
+      <c r="G48" s="26" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="49" spans="3:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C49" s="25"/>
-      <c r="D49" s="26"/>
-      <c r="E49" s="27"/>
-      <c r="F49" s="19" t="s">
-        <v>16</v>
-      </c>
-      <c r="G49" s="20" t="s">
+    <row r="49" spans="3:7" ht="15" customHeight="1" thickBot="1">
+      <c r="C49" s="22"/>
+      <c r="D49" s="23"/>
+      <c r="E49" s="24"/>
+      <c r="F49" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="G49" s="26" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="50" spans="3:7" ht="3" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C50" s="14"/>
-      <c r="D50" s="15"/>
-      <c r="E50" s="16"/>
-      <c r="F50" s="17"/>
-      <c r="G50" s="18"/>
-    </row>
-    <row r="51" spans="3:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C51" s="25" t="s">
+    <row r="50" spans="3:7" ht="3" customHeight="1" thickBot="1">
+      <c r="C50" s="17"/>
+      <c r="D50" s="18"/>
+      <c r="E50" s="19"/>
+      <c r="F50" s="20"/>
+      <c r="G50" s="21"/>
+    </row>
+    <row r="51" spans="3:7" ht="15" customHeight="1" thickBot="1">
+      <c r="C51" s="22" t="s">
         <v>65</v>
       </c>
-      <c r="D51" s="26" t="s">
+      <c r="D51" s="23" t="s">
         <v>66</v>
       </c>
-      <c r="E51" s="27" t="s">
+      <c r="E51" s="24" t="s">
         <v>66</v>
       </c>
-      <c r="F51" s="19" t="s">
-        <v>14</v>
-      </c>
-      <c r="G51" s="20" t="s">
+      <c r="F51" s="25" t="s">
+        <v>14</v>
+      </c>
+      <c r="G51" s="26" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="52" spans="3:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C52" s="25"/>
-      <c r="D52" s="26"/>
-      <c r="E52" s="27"/>
-      <c r="F52" s="19" t="s">
-        <v>16</v>
-      </c>
-      <c r="G52" s="20" t="s">
+    <row r="52" spans="3:7" ht="15" customHeight="1" thickBot="1">
+      <c r="C52" s="22"/>
+      <c r="D52" s="23"/>
+      <c r="E52" s="24"/>
+      <c r="F52" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="G52" s="26" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="53" spans="3:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C53" s="21"/>
-      <c r="D53" s="22"/>
-      <c r="E53" s="22"/>
-      <c r="F53" s="23"/>
-      <c r="G53" s="24"/>
-    </row>
-    <row r="54" spans="3:7" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C54" s="11" t="s">
+    <row r="53" spans="3:7" ht="14.4" thickBot="1">
+      <c r="C53" s="27"/>
+      <c r="D53" s="28"/>
+      <c r="E53" s="28"/>
+      <c r="F53" s="29"/>
+      <c r="G53" s="30"/>
+    </row>
+    <row r="54" spans="3:7" ht="27.75" customHeight="1" thickBot="1">
+      <c r="C54" s="12" t="s">
         <v>68</v>
       </c>
-      <c r="D54" s="12" t="s">
+      <c r="D54" s="13" t="s">
         <v>69</v>
       </c>
-      <c r="E54" s="13" t="s">
+      <c r="E54" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="F54" s="28" t="s">
+      <c r="F54" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="G54" s="29"/>
-    </row>
-    <row r="55" spans="3:7" ht="3" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C55" s="14"/>
-      <c r="D55" s="15"/>
-      <c r="E55" s="16"/>
-      <c r="F55" s="17"/>
-      <c r="G55" s="18"/>
-    </row>
-    <row r="56" spans="3:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C56" s="25" t="s">
+      <c r="G54" s="16"/>
+    </row>
+    <row r="55" spans="3:7" ht="3" customHeight="1" thickBot="1">
+      <c r="C55" s="17"/>
+      <c r="D55" s="18"/>
+      <c r="E55" s="19"/>
+      <c r="F55" s="20"/>
+      <c r="G55" s="21"/>
+    </row>
+    <row r="56" spans="3:7" ht="15" customHeight="1" thickBot="1">
+      <c r="C56" s="22" t="s">
         <v>70</v>
       </c>
-      <c r="D56" s="26" t="s">
+      <c r="D56" s="23" t="s">
         <v>71</v>
       </c>
-      <c r="E56" s="27" t="s">
+      <c r="E56" s="24" t="s">
         <v>71</v>
       </c>
-      <c r="F56" s="19" t="s">
-        <v>14</v>
-      </c>
-      <c r="G56" s="20" t="s">
+      <c r="F56" s="25" t="s">
+        <v>14</v>
+      </c>
+      <c r="G56" s="26" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="57" spans="3:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C57" s="25"/>
-      <c r="D57" s="26"/>
-      <c r="E57" s="27"/>
-      <c r="F57" s="19" t="s">
-        <v>16</v>
-      </c>
-      <c r="G57" s="20" t="s">
+    <row r="57" spans="3:7" ht="15" customHeight="1" thickBot="1">
+      <c r="C57" s="22"/>
+      <c r="D57" s="23"/>
+      <c r="E57" s="24"/>
+      <c r="F57" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="G57" s="26" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="58" spans="3:7" ht="3" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C58" s="14"/>
-      <c r="D58" s="15"/>
-      <c r="E58" s="16"/>
-      <c r="F58" s="17"/>
-      <c r="G58" s="18"/>
-    </row>
-    <row r="59" spans="3:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C59" s="25" t="s">
+    <row r="58" spans="3:7" ht="3" customHeight="1" thickBot="1">
+      <c r="C58" s="17"/>
+      <c r="D58" s="18"/>
+      <c r="E58" s="19"/>
+      <c r="F58" s="20"/>
+      <c r="G58" s="21"/>
+    </row>
+    <row r="59" spans="3:7" ht="15" customHeight="1" thickBot="1">
+      <c r="C59" s="22" t="s">
         <v>73</v>
       </c>
-      <c r="D59" s="26" t="s">
+      <c r="D59" s="23" t="s">
         <v>74</v>
       </c>
-      <c r="E59" s="27" t="s">
+      <c r="E59" s="24" t="s">
         <v>75</v>
       </c>
-      <c r="F59" s="19" t="s">
-        <v>14</v>
-      </c>
-      <c r="G59" s="20" t="s">
+      <c r="F59" s="25" t="s">
+        <v>14</v>
+      </c>
+      <c r="G59" s="26" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="60" spans="3:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C60" s="25"/>
-      <c r="D60" s="26"/>
-      <c r="E60" s="27"/>
-      <c r="F60" s="19" t="s">
-        <v>16</v>
-      </c>
-      <c r="G60" s="20" t="s">
+    <row r="60" spans="3:7" ht="15" customHeight="1" thickBot="1">
+      <c r="C60" s="22"/>
+      <c r="D60" s="23"/>
+      <c r="E60" s="24"/>
+      <c r="F60" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="G60" s="26" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="61" spans="3:7" ht="3" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C61" s="14"/>
-      <c r="D61" s="15"/>
-      <c r="E61" s="16"/>
-      <c r="F61" s="17"/>
-      <c r="G61" s="18"/>
-    </row>
-    <row r="62" spans="3:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C62" s="25" t="s">
+    <row r="61" spans="3:7" ht="3" customHeight="1" thickBot="1">
+      <c r="C61" s="17"/>
+      <c r="D61" s="18"/>
+      <c r="E61" s="19"/>
+      <c r="F61" s="20"/>
+      <c r="G61" s="21"/>
+    </row>
+    <row r="62" spans="3:7" ht="15" customHeight="1" thickBot="1">
+      <c r="C62" s="22" t="s">
         <v>76</v>
       </c>
-      <c r="D62" s="26" t="s">
+      <c r="D62" s="23" t="s">
         <v>77</v>
       </c>
-      <c r="E62" s="27" t="s">
+      <c r="E62" s="24" t="s">
         <v>77</v>
       </c>
-      <c r="F62" s="19" t="s">
-        <v>14</v>
-      </c>
-      <c r="G62" s="20" t="s">
+      <c r="F62" s="25" t="s">
+        <v>14</v>
+      </c>
+      <c r="G62" s="26" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="63" spans="3:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C63" s="25"/>
-      <c r="D63" s="26"/>
-      <c r="E63" s="27"/>
-      <c r="F63" s="19" t="s">
-        <v>16</v>
-      </c>
-      <c r="G63" s="20" t="s">
+    <row r="63" spans="3:7" ht="15" customHeight="1" thickBot="1">
+      <c r="C63" s="22"/>
+      <c r="D63" s="23"/>
+      <c r="E63" s="24"/>
+      <c r="F63" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="G63" s="26" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="64" spans="3:7" ht="3" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C64" s="14"/>
-      <c r="D64" s="15"/>
-      <c r="E64" s="16"/>
-      <c r="F64" s="17"/>
-      <c r="G64" s="18"/>
-    </row>
-    <row r="65" spans="3:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C65" s="25" t="s">
+    <row r="64" spans="3:7" ht="3" customHeight="1" thickBot="1">
+      <c r="C64" s="17"/>
+      <c r="D64" s="18"/>
+      <c r="E64" s="19"/>
+      <c r="F64" s="20"/>
+      <c r="G64" s="21"/>
+    </row>
+    <row r="65" spans="3:7" ht="15" customHeight="1" thickBot="1">
+      <c r="C65" s="22" t="s">
         <v>78</v>
       </c>
-      <c r="D65" s="26" t="s">
+      <c r="D65" s="23" t="s">
         <v>79</v>
       </c>
-      <c r="E65" s="27" t="s">
+      <c r="E65" s="24" t="s">
         <v>79</v>
       </c>
-      <c r="F65" s="19" t="s">
-        <v>14</v>
-      </c>
-      <c r="G65" s="20" t="s">
+      <c r="F65" s="25" t="s">
+        <v>14</v>
+      </c>
+      <c r="G65" s="26" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="66" spans="3:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C66" s="25"/>
-      <c r="D66" s="26"/>
-      <c r="E66" s="27"/>
-      <c r="F66" s="19" t="s">
-        <v>16</v>
-      </c>
-      <c r="G66" s="20" t="s">
+    <row r="66" spans="3:7" ht="15" customHeight="1" thickBot="1">
+      <c r="C66" s="22"/>
+      <c r="D66" s="23"/>
+      <c r="E66" s="24"/>
+      <c r="F66" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="G66" s="26" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="67" spans="3:7" ht="3" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C67" s="14"/>
-      <c r="D67" s="15"/>
-      <c r="E67" s="16"/>
-      <c r="F67" s="17"/>
-      <c r="G67" s="18"/>
-    </row>
-    <row r="68" spans="3:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C68" s="25" t="s">
+    <row r="67" spans="3:7" ht="3" customHeight="1" thickBot="1">
+      <c r="C67" s="17"/>
+      <c r="D67" s="18"/>
+      <c r="E67" s="19"/>
+      <c r="F67" s="20"/>
+      <c r="G67" s="21"/>
+    </row>
+    <row r="68" spans="3:7" ht="15" customHeight="1" thickBot="1">
+      <c r="C68" s="22" t="s">
         <v>81</v>
       </c>
-      <c r="D68" s="26" t="s">
+      <c r="D68" s="23" t="s">
         <v>82</v>
       </c>
-      <c r="E68" s="27" t="s">
+      <c r="E68" s="24" t="s">
         <v>82</v>
       </c>
-      <c r="F68" s="19" t="s">
-        <v>14</v>
-      </c>
-      <c r="G68" s="20" t="s">
+      <c r="F68" s="25" t="s">
+        <v>14</v>
+      </c>
+      <c r="G68" s="26" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="69" spans="3:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C69" s="25"/>
-      <c r="D69" s="26"/>
-      <c r="E69" s="27"/>
-      <c r="F69" s="19" t="s">
-        <v>16</v>
-      </c>
-      <c r="G69" s="20" t="s">
+    <row r="69" spans="3:7" ht="15" customHeight="1" thickBot="1">
+      <c r="C69" s="22"/>
+      <c r="D69" s="23"/>
+      <c r="E69" s="24"/>
+      <c r="F69" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="G69" s="26" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="70" spans="3:7" ht="3" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C70" s="14"/>
-      <c r="D70" s="15"/>
-      <c r="E70" s="16"/>
-      <c r="F70" s="17"/>
-      <c r="G70" s="18"/>
-    </row>
-    <row r="71" spans="3:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C71" s="25" t="s">
+    <row r="70" spans="3:7" ht="3" customHeight="1" thickBot="1">
+      <c r="C70" s="17"/>
+      <c r="D70" s="18"/>
+      <c r="E70" s="19"/>
+      <c r="F70" s="20"/>
+      <c r="G70" s="21"/>
+    </row>
+    <row r="71" spans="3:7" ht="15" customHeight="1" thickBot="1">
+      <c r="C71" s="22" t="s">
         <v>83</v>
       </c>
-      <c r="D71" s="26" t="s">
+      <c r="D71" s="23" t="s">
         <v>84</v>
       </c>
-      <c r="E71" s="27" t="s">
+      <c r="E71" s="24" t="s">
         <v>84</v>
       </c>
-      <c r="F71" s="19" t="s">
-        <v>14</v>
-      </c>
-      <c r="G71" s="20" t="s">
+      <c r="F71" s="25" t="s">
+        <v>14</v>
+      </c>
+      <c r="G71" s="26" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="72" spans="3:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C72" s="25"/>
-      <c r="D72" s="26"/>
-      <c r="E72" s="27"/>
-      <c r="F72" s="19" t="s">
-        <v>16</v>
-      </c>
-      <c r="G72" s="20" t="s">
+    <row r="72" spans="3:7" ht="15" customHeight="1" thickBot="1">
+      <c r="C72" s="22"/>
+      <c r="D72" s="23"/>
+      <c r="E72" s="24"/>
+      <c r="F72" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="G72" s="26" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="73" spans="3:7" ht="3" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C73" s="14"/>
-      <c r="D73" s="15"/>
-      <c r="E73" s="16"/>
-      <c r="F73" s="17"/>
-      <c r="G73" s="18"/>
-    </row>
-    <row r="74" spans="3:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C74" s="25" t="s">
+    <row r="73" spans="3:7" ht="3" customHeight="1" thickBot="1">
+      <c r="C73" s="17"/>
+      <c r="D73" s="18"/>
+      <c r="E73" s="19"/>
+      <c r="F73" s="20"/>
+      <c r="G73" s="21"/>
+    </row>
+    <row r="74" spans="3:7" ht="15" customHeight="1" thickBot="1">
+      <c r="C74" s="22" t="s">
         <v>85</v>
       </c>
-      <c r="D74" s="26" t="s">
+      <c r="D74" s="23" t="s">
         <v>86</v>
       </c>
-      <c r="E74" s="27" t="s">
+      <c r="E74" s="24" t="s">
         <v>86</v>
       </c>
-      <c r="F74" s="19" t="s">
-        <v>14</v>
-      </c>
-      <c r="G74" s="20" t="s">
+      <c r="F74" s="25" t="s">
+        <v>14</v>
+      </c>
+      <c r="G74" s="26" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="75" spans="3:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C75" s="25"/>
-      <c r="D75" s="26"/>
-      <c r="E75" s="27"/>
-      <c r="F75" s="19" t="s">
-        <v>16</v>
-      </c>
-      <c r="G75" s="20" t="s">
+    <row r="75" spans="3:7" ht="15" customHeight="1" thickBot="1">
+      <c r="C75" s="22"/>
+      <c r="D75" s="23"/>
+      <c r="E75" s="24"/>
+      <c r="F75" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="G75" s="26" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="76" spans="3:7" ht="3" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C76" s="14"/>
-      <c r="D76" s="15"/>
-      <c r="E76" s="16"/>
-      <c r="F76" s="17"/>
-      <c r="G76" s="18"/>
-    </row>
-    <row r="77" spans="3:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C77" s="25" t="s">
+    <row r="76" spans="3:7" ht="3" customHeight="1" thickBot="1">
+      <c r="C76" s="17"/>
+      <c r="D76" s="18"/>
+      <c r="E76" s="19"/>
+      <c r="F76" s="20"/>
+      <c r="G76" s="21"/>
+    </row>
+    <row r="77" spans="3:7" ht="15" customHeight="1" thickBot="1">
+      <c r="C77" s="22" t="s">
         <v>87</v>
       </c>
-      <c r="D77" s="26" t="s">
+      <c r="D77" s="23" t="s">
         <v>88</v>
       </c>
-      <c r="E77" s="27" t="s">
+      <c r="E77" s="24" t="s">
         <v>89</v>
       </c>
-      <c r="F77" s="19" t="s">
-        <v>14</v>
-      </c>
-      <c r="G77" s="20" t="s">
+      <c r="F77" s="25" t="s">
+        <v>14</v>
+      </c>
+      <c r="G77" s="26" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="78" spans="3:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C78" s="25"/>
-      <c r="D78" s="26"/>
-      <c r="E78" s="27"/>
-      <c r="F78" s="19" t="s">
-        <v>16</v>
-      </c>
-      <c r="G78" s="20" t="s">
+    <row r="78" spans="3:7" ht="15" customHeight="1" thickBot="1">
+      <c r="C78" s="22"/>
+      <c r="D78" s="23"/>
+      <c r="E78" s="24"/>
+      <c r="F78" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="G78" s="26" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="79" spans="3:7" ht="3" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C79" s="14"/>
-      <c r="D79" s="15"/>
-      <c r="E79" s="16"/>
-      <c r="F79" s="17"/>
-      <c r="G79" s="18"/>
-    </row>
-    <row r="80" spans="3:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C80" s="25" t="s">
+    <row r="79" spans="3:7" ht="3" customHeight="1" thickBot="1">
+      <c r="C79" s="17"/>
+      <c r="D79" s="18"/>
+      <c r="E79" s="19"/>
+      <c r="F79" s="20"/>
+      <c r="G79" s="21"/>
+    </row>
+    <row r="80" spans="3:7" ht="15" customHeight="1" thickBot="1">
+      <c r="C80" s="22" t="s">
         <v>91</v>
       </c>
-      <c r="D80" s="26" t="s">
+      <c r="D80" s="23" t="s">
         <v>92</v>
       </c>
-      <c r="E80" s="27" t="s">
+      <c r="E80" s="24" t="s">
         <v>93</v>
       </c>
-      <c r="F80" s="19" t="s">
-        <v>14</v>
-      </c>
-      <c r="G80" s="20" t="s">
+      <c r="F80" s="25" t="s">
+        <v>14</v>
+      </c>
+      <c r="G80" s="26" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="81" spans="3:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C81" s="25"/>
-      <c r="D81" s="26"/>
-      <c r="E81" s="27"/>
-      <c r="F81" s="19" t="s">
-        <v>16</v>
-      </c>
-      <c r="G81" s="20" t="s">
+    <row r="81" spans="3:7" ht="15" customHeight="1" thickBot="1">
+      <c r="C81" s="22"/>
+      <c r="D81" s="23"/>
+      <c r="E81" s="24"/>
+      <c r="F81" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="G81" s="26" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="82" spans="3:7" ht="3" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C82" s="14"/>
-      <c r="D82" s="15"/>
-      <c r="E82" s="16"/>
-      <c r="F82" s="17"/>
-      <c r="G82" s="18"/>
-    </row>
-    <row r="83" spans="3:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C83" s="25" t="s">
+    <row r="82" spans="3:7" ht="3" customHeight="1" thickBot="1">
+      <c r="C82" s="17"/>
+      <c r="D82" s="18"/>
+      <c r="E82" s="19"/>
+      <c r="F82" s="20"/>
+      <c r="G82" s="21"/>
+    </row>
+    <row r="83" spans="3:7" ht="15" customHeight="1" thickBot="1">
+      <c r="C83" s="22" t="s">
         <v>94</v>
       </c>
-      <c r="D83" s="26" t="s">
+      <c r="D83" s="23" t="s">
         <v>95</v>
       </c>
-      <c r="E83" s="27" t="s">
+      <c r="E83" s="24" t="s">
         <v>96</v>
       </c>
-      <c r="F83" s="19" t="s">
-        <v>14</v>
-      </c>
-      <c r="G83" s="20" t="s">
+      <c r="F83" s="25" t="s">
+        <v>14</v>
+      </c>
+      <c r="G83" s="26" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="84" spans="3:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C84" s="25"/>
-      <c r="D84" s="26"/>
-      <c r="E84" s="27"/>
-      <c r="F84" s="19" t="s">
-        <v>16</v>
-      </c>
-      <c r="G84" s="20" t="s">
+    <row r="84" spans="3:7" ht="15" customHeight="1" thickBot="1">
+      <c r="C84" s="22"/>
+      <c r="D84" s="23"/>
+      <c r="E84" s="24"/>
+      <c r="F84" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="G84" s="26" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="85" spans="3:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C85" s="21"/>
-      <c r="D85" s="22"/>
-      <c r="E85" s="22"/>
-      <c r="F85" s="23"/>
-      <c r="G85" s="24"/>
-    </row>
-    <row r="86" spans="3:7" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C86" s="11" t="s">
+    <row r="85" spans="3:7" ht="14.4" thickBot="1">
+      <c r="C85" s="27"/>
+      <c r="D85" s="28"/>
+      <c r="E85" s="28"/>
+      <c r="F85" s="29"/>
+      <c r="G85" s="30"/>
+    </row>
+    <row r="86" spans="3:7" ht="27.75" customHeight="1" thickBot="1">
+      <c r="C86" s="12" t="s">
         <v>98</v>
       </c>
-      <c r="D86" s="12" t="s">
+      <c r="D86" s="13" t="s">
         <v>99</v>
       </c>
-      <c r="E86" s="13" t="s">
+      <c r="E86" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="F86" s="28" t="s">
+      <c r="F86" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="G86" s="29"/>
-    </row>
-    <row r="87" spans="3:7" ht="3" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C87" s="14"/>
-      <c r="D87" s="15"/>
-      <c r="E87" s="16"/>
-      <c r="F87" s="17"/>
-      <c r="G87" s="18"/>
-    </row>
-    <row r="88" spans="3:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C88" s="25" t="s">
+      <c r="G86" s="16"/>
+    </row>
+    <row r="87" spans="3:7" ht="3" customHeight="1" thickBot="1">
+      <c r="C87" s="17"/>
+      <c r="D87" s="18"/>
+      <c r="E87" s="19"/>
+      <c r="F87" s="20"/>
+      <c r="G87" s="21"/>
+    </row>
+    <row r="88" spans="3:7" ht="15" customHeight="1" thickBot="1">
+      <c r="C88" s="22" t="s">
         <v>100</v>
       </c>
-      <c r="D88" s="26" t="s">
+      <c r="D88" s="23" t="s">
         <v>101</v>
       </c>
-      <c r="E88" s="27" t="s">
+      <c r="E88" s="24" t="s">
         <v>102</v>
       </c>
-      <c r="F88" s="19" t="s">
-        <v>14</v>
-      </c>
-      <c r="G88" s="20" t="s">
+      <c r="F88" s="25" t="s">
+        <v>14</v>
+      </c>
+      <c r="G88" s="26" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="89" spans="3:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C89" s="25"/>
-      <c r="D89" s="26"/>
-      <c r="E89" s="27"/>
-      <c r="F89" s="19" t="s">
-        <v>16</v>
-      </c>
-      <c r="G89" s="20" t="s">
+    <row r="89" spans="3:7" ht="15" customHeight="1" thickBot="1">
+      <c r="C89" s="22"/>
+      <c r="D89" s="23"/>
+      <c r="E89" s="24"/>
+      <c r="F89" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="G89" s="26" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="90" spans="3:7" ht="3" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C90" s="14"/>
-      <c r="D90" s="15"/>
-      <c r="E90" s="16"/>
-      <c r="F90" s="17"/>
-      <c r="G90" s="18"/>
-    </row>
-    <row r="91" spans="3:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C91" s="25" t="s">
+    <row r="90" spans="3:7" ht="3" customHeight="1" thickBot="1">
+      <c r="C90" s="17"/>
+      <c r="D90" s="18"/>
+      <c r="E90" s="19"/>
+      <c r="F90" s="20"/>
+      <c r="G90" s="21"/>
+    </row>
+    <row r="91" spans="3:7" ht="15" customHeight="1" thickBot="1">
+      <c r="C91" s="22" t="s">
         <v>103</v>
       </c>
-      <c r="D91" s="26" t="s">
+      <c r="D91" s="23" t="s">
         <v>104</v>
       </c>
-      <c r="E91" s="27" t="s">
+      <c r="E91" s="24" t="s">
         <v>105</v>
       </c>
-      <c r="F91" s="19" t="s">
-        <v>14</v>
-      </c>
-      <c r="G91" s="20" t="s">
+      <c r="F91" s="25" t="s">
+        <v>14</v>
+      </c>
+      <c r="G91" s="26" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="92" spans="3:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C92" s="25"/>
-      <c r="D92" s="26"/>
-      <c r="E92" s="27"/>
-      <c r="F92" s="19" t="s">
-        <v>16</v>
-      </c>
-      <c r="G92" s="20" t="s">
+    <row r="92" spans="3:7" ht="15" customHeight="1" thickBot="1">
+      <c r="C92" s="22"/>
+      <c r="D92" s="23"/>
+      <c r="E92" s="24"/>
+      <c r="F92" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="G92" s="26" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="93" spans="3:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C93" s="21"/>
-      <c r="D93" s="22"/>
-      <c r="E93" s="22"/>
-      <c r="F93" s="23"/>
-      <c r="G93" s="24"/>
-    </row>
-    <row r="94" spans="3:7" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C94" s="11" t="s">
+    <row r="93" spans="3:7" ht="14.4" thickBot="1">
+      <c r="C93" s="27"/>
+      <c r="D93" s="28"/>
+      <c r="E93" s="28"/>
+      <c r="F93" s="29"/>
+      <c r="G93" s="30"/>
+    </row>
+    <row r="94" spans="3:7" ht="27.75" customHeight="1" thickBot="1">
+      <c r="C94" s="12" t="s">
         <v>107</v>
       </c>
-      <c r="D94" s="12" t="s">
+      <c r="D94" s="13" t="s">
         <v>108</v>
       </c>
-      <c r="E94" s="13" t="s">
+      <c r="E94" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="F94" s="28" t="s">
+      <c r="F94" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="G94" s="29"/>
-    </row>
-    <row r="95" spans="3:7" ht="3" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C95" s="14"/>
-      <c r="D95" s="15"/>
-      <c r="E95" s="16"/>
-      <c r="F95" s="17"/>
-      <c r="G95" s="18"/>
-    </row>
-    <row r="96" spans="3:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C96" s="25" t="s">
+      <c r="G94" s="16"/>
+    </row>
+    <row r="95" spans="3:7" ht="3" customHeight="1" thickBot="1">
+      <c r="C95" s="17"/>
+      <c r="D95" s="18"/>
+      <c r="E95" s="19"/>
+      <c r="F95" s="20"/>
+      <c r="G95" s="21"/>
+    </row>
+    <row r="96" spans="3:7" ht="15" customHeight="1" thickBot="1">
+      <c r="C96" s="22" t="s">
         <v>109</v>
       </c>
-      <c r="D96" s="26" t="s">
+      <c r="D96" s="23" t="s">
         <v>110</v>
       </c>
-      <c r="E96" s="27" t="s">
+      <c r="E96" s="24" t="s">
         <v>110</v>
       </c>
-      <c r="F96" s="19" t="s">
-        <v>14</v>
-      </c>
-      <c r="G96" s="20" t="s">
+      <c r="F96" s="25" t="s">
+        <v>14</v>
+      </c>
+      <c r="G96" s="26" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="97" spans="3:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C97" s="25"/>
-      <c r="D97" s="26"/>
-      <c r="E97" s="27"/>
-      <c r="F97" s="19" t="s">
-        <v>16</v>
-      </c>
-      <c r="G97" s="20" t="s">
+    <row r="97" spans="3:7" ht="15" customHeight="1" thickBot="1">
+      <c r="C97" s="22"/>
+      <c r="D97" s="23"/>
+      <c r="E97" s="24"/>
+      <c r="F97" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="G97" s="26" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="98" spans="3:7" ht="3" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C98" s="14"/>
-      <c r="D98" s="15"/>
-      <c r="E98" s="16"/>
-      <c r="F98" s="17"/>
-      <c r="G98" s="18"/>
-    </row>
-    <row r="99" spans="3:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C99" s="25" t="s">
+    <row r="98" spans="3:7" ht="3" customHeight="1" thickBot="1">
+      <c r="C98" s="17"/>
+      <c r="D98" s="18"/>
+      <c r="E98" s="19"/>
+      <c r="F98" s="20"/>
+      <c r="G98" s="21"/>
+    </row>
+    <row r="99" spans="3:7" ht="15" customHeight="1" thickBot="1">
+      <c r="C99" s="22" t="s">
         <v>112</v>
       </c>
-      <c r="D99" s="26" t="s">
+      <c r="D99" s="23" t="s">
         <v>113</v>
       </c>
-      <c r="E99" s="27" t="s">
+      <c r="E99" s="24" t="s">
         <v>113</v>
       </c>
-      <c r="F99" s="19" t="s">
-        <v>14</v>
-      </c>
-      <c r="G99" s="20" t="s">
+      <c r="F99" s="25" t="s">
+        <v>14</v>
+      </c>
+      <c r="G99" s="26" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="100" spans="3:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C100" s="25"/>
-      <c r="D100" s="26"/>
-      <c r="E100" s="27"/>
-      <c r="F100" s="19" t="s">
-        <v>16</v>
-      </c>
-      <c r="G100" s="20" t="s">
+    <row r="100" spans="3:7" ht="15" customHeight="1" thickBot="1">
+      <c r="C100" s="22"/>
+      <c r="D100" s="23"/>
+      <c r="E100" s="24"/>
+      <c r="F100" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="G100" s="26" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="101" spans="3:7" ht="3" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C101" s="14"/>
-      <c r="D101" s="15"/>
-      <c r="E101" s="16"/>
-      <c r="F101" s="17"/>
-      <c r="G101" s="18"/>
-    </row>
-    <row r="102" spans="3:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C102" s="25" t="s">
+    <row r="101" spans="3:7" ht="3" customHeight="1" thickBot="1">
+      <c r="C101" s="17"/>
+      <c r="D101" s="18"/>
+      <c r="E101" s="19"/>
+      <c r="F101" s="20"/>
+      <c r="G101" s="21"/>
+    </row>
+    <row r="102" spans="3:7" ht="15" customHeight="1" thickBot="1">
+      <c r="C102" s="22" t="s">
         <v>115</v>
       </c>
-      <c r="D102" s="26" t="s">
+      <c r="D102" s="23" t="s">
         <v>116</v>
       </c>
-      <c r="E102" s="27" t="s">
+      <c r="E102" s="24" t="s">
         <v>116</v>
       </c>
-      <c r="F102" s="19" t="s">
-        <v>14</v>
-      </c>
-      <c r="G102" s="20" t="s">
+      <c r="F102" s="25" t="s">
+        <v>14</v>
+      </c>
+      <c r="G102" s="26" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="103" spans="3:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C103" s="25"/>
-      <c r="D103" s="26"/>
-      <c r="E103" s="27"/>
-      <c r="F103" s="19" t="s">
-        <v>16</v>
-      </c>
-      <c r="G103" s="20" t="s">
+    <row r="103" spans="3:7" ht="15" customHeight="1" thickBot="1">
+      <c r="C103" s="22"/>
+      <c r="D103" s="23"/>
+      <c r="E103" s="24"/>
+      <c r="F103" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="G103" s="26" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="104" spans="3:7" ht="3" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C104" s="14"/>
-      <c r="D104" s="15"/>
-      <c r="E104" s="16"/>
-      <c r="F104" s="17"/>
-      <c r="G104" s="18"/>
-    </row>
-    <row r="105" spans="3:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C105" s="25" t="s">
+    <row r="104" spans="3:7" ht="3" customHeight="1" thickBot="1">
+      <c r="C104" s="17"/>
+      <c r="D104" s="18"/>
+      <c r="E104" s="19"/>
+      <c r="F104" s="20"/>
+      <c r="G104" s="21"/>
+    </row>
+    <row r="105" spans="3:7" ht="15" customHeight="1" thickBot="1">
+      <c r="C105" s="22" t="s">
         <v>118</v>
       </c>
-      <c r="D105" s="26" t="s">
+      <c r="D105" s="23" t="s">
         <v>119</v>
       </c>
-      <c r="E105" s="27" t="s">
+      <c r="E105" s="24" t="s">
         <v>119</v>
       </c>
-      <c r="F105" s="19" t="s">
-        <v>14</v>
-      </c>
-      <c r="G105" s="20" t="s">
+      <c r="F105" s="25" t="s">
+        <v>14</v>
+      </c>
+      <c r="G105" s="26" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="106" spans="3:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C106" s="25"/>
-      <c r="D106" s="26"/>
-      <c r="E106" s="27"/>
-      <c r="F106" s="19" t="s">
-        <v>16</v>
-      </c>
-      <c r="G106" s="20" t="s">
+    <row r="106" spans="3:7" ht="15" customHeight="1" thickBot="1">
+      <c r="C106" s="22"/>
+      <c r="D106" s="23"/>
+      <c r="E106" s="24"/>
+      <c r="F106" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="G106" s="26" t="s">
         <v>57</v>
       </c>
     </row>
   </sheetData>
   <sheetProtection password="A790" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="93">
-    <mergeCell ref="C16:C17"/>
-    <mergeCell ref="D16:D17"/>
-    <mergeCell ref="E16:E17"/>
-    <mergeCell ref="C2:G4"/>
-    <mergeCell ref="F11:G11"/>
-    <mergeCell ref="C13:C14"/>
-    <mergeCell ref="D13:D14"/>
-    <mergeCell ref="E13:E14"/>
-    <mergeCell ref="C19:C20"/>
-    <mergeCell ref="D19:D20"/>
-    <mergeCell ref="E19:E20"/>
-    <mergeCell ref="C22:C23"/>
-    <mergeCell ref="D22:D23"/>
-    <mergeCell ref="E22:E23"/>
-    <mergeCell ref="C25:C26"/>
-    <mergeCell ref="D25:D26"/>
-    <mergeCell ref="E25:E26"/>
-    <mergeCell ref="C28:C29"/>
-    <mergeCell ref="D28:D29"/>
-    <mergeCell ref="E28:E29"/>
-    <mergeCell ref="F31:G31"/>
-    <mergeCell ref="C33:C34"/>
-    <mergeCell ref="D33:D34"/>
-    <mergeCell ref="E33:E34"/>
-    <mergeCell ref="C36:C37"/>
-    <mergeCell ref="D36:D37"/>
-    <mergeCell ref="E36:E37"/>
-    <mergeCell ref="C39:C40"/>
-    <mergeCell ref="D39:D40"/>
-    <mergeCell ref="E39:E40"/>
-    <mergeCell ref="C42:C43"/>
-    <mergeCell ref="D42:D43"/>
-    <mergeCell ref="E42:E43"/>
-    <mergeCell ref="C45:C46"/>
-    <mergeCell ref="D45:D46"/>
-    <mergeCell ref="E45:E46"/>
-    <mergeCell ref="C48:C49"/>
-    <mergeCell ref="D48:D49"/>
-    <mergeCell ref="E48:E49"/>
-    <mergeCell ref="C51:C52"/>
-    <mergeCell ref="D51:D52"/>
-    <mergeCell ref="E51:E52"/>
-    <mergeCell ref="F54:G54"/>
-    <mergeCell ref="C56:C57"/>
-    <mergeCell ref="D56:D57"/>
-    <mergeCell ref="E56:E57"/>
-    <mergeCell ref="C59:C60"/>
-    <mergeCell ref="D59:D60"/>
-    <mergeCell ref="E59:E60"/>
-    <mergeCell ref="C62:C63"/>
-    <mergeCell ref="D62:D63"/>
-    <mergeCell ref="E62:E63"/>
-    <mergeCell ref="C65:C66"/>
-    <mergeCell ref="D65:D66"/>
-    <mergeCell ref="E65:E66"/>
-    <mergeCell ref="C68:C69"/>
-    <mergeCell ref="D68:D69"/>
-    <mergeCell ref="E68:E69"/>
-    <mergeCell ref="C71:C72"/>
-    <mergeCell ref="D71:D72"/>
-    <mergeCell ref="E71:E72"/>
-    <mergeCell ref="C74:C75"/>
-    <mergeCell ref="D74:D75"/>
-    <mergeCell ref="E74:E75"/>
-    <mergeCell ref="C77:C78"/>
-    <mergeCell ref="D77:D78"/>
-    <mergeCell ref="E77:E78"/>
-    <mergeCell ref="C80:C81"/>
-    <mergeCell ref="D80:D81"/>
-    <mergeCell ref="E80:E81"/>
-    <mergeCell ref="C83:C84"/>
-    <mergeCell ref="D83:D84"/>
-    <mergeCell ref="E83:E84"/>
-    <mergeCell ref="F86:G86"/>
-    <mergeCell ref="C88:C89"/>
-    <mergeCell ref="D88:D89"/>
-    <mergeCell ref="E88:E89"/>
-    <mergeCell ref="C91:C92"/>
-    <mergeCell ref="D91:D92"/>
-    <mergeCell ref="E91:E92"/>
-    <mergeCell ref="F94:G94"/>
-    <mergeCell ref="C96:C97"/>
-    <mergeCell ref="D96:D97"/>
-    <mergeCell ref="E96:E97"/>
     <mergeCell ref="C105:C106"/>
     <mergeCell ref="D105:D106"/>
     <mergeCell ref="E105:E106"/>
@@ -2543,6 +2472,90 @@
     <mergeCell ref="C102:C103"/>
     <mergeCell ref="D102:D103"/>
     <mergeCell ref="E102:E103"/>
+    <mergeCell ref="C91:C92"/>
+    <mergeCell ref="D91:D92"/>
+    <mergeCell ref="E91:E92"/>
+    <mergeCell ref="F94:G94"/>
+    <mergeCell ref="C96:C97"/>
+    <mergeCell ref="D96:D97"/>
+    <mergeCell ref="E96:E97"/>
+    <mergeCell ref="C83:C84"/>
+    <mergeCell ref="D83:D84"/>
+    <mergeCell ref="E83:E84"/>
+    <mergeCell ref="F86:G86"/>
+    <mergeCell ref="C88:C89"/>
+    <mergeCell ref="D88:D89"/>
+    <mergeCell ref="E88:E89"/>
+    <mergeCell ref="C77:C78"/>
+    <mergeCell ref="D77:D78"/>
+    <mergeCell ref="E77:E78"/>
+    <mergeCell ref="C80:C81"/>
+    <mergeCell ref="D80:D81"/>
+    <mergeCell ref="E80:E81"/>
+    <mergeCell ref="C71:C72"/>
+    <mergeCell ref="D71:D72"/>
+    <mergeCell ref="E71:E72"/>
+    <mergeCell ref="C74:C75"/>
+    <mergeCell ref="D74:D75"/>
+    <mergeCell ref="E74:E75"/>
+    <mergeCell ref="C65:C66"/>
+    <mergeCell ref="D65:D66"/>
+    <mergeCell ref="E65:E66"/>
+    <mergeCell ref="C68:C69"/>
+    <mergeCell ref="D68:D69"/>
+    <mergeCell ref="E68:E69"/>
+    <mergeCell ref="C59:C60"/>
+    <mergeCell ref="D59:D60"/>
+    <mergeCell ref="E59:E60"/>
+    <mergeCell ref="C62:C63"/>
+    <mergeCell ref="D62:D63"/>
+    <mergeCell ref="E62:E63"/>
+    <mergeCell ref="C51:C52"/>
+    <mergeCell ref="D51:D52"/>
+    <mergeCell ref="E51:E52"/>
+    <mergeCell ref="F54:G54"/>
+    <mergeCell ref="C56:C57"/>
+    <mergeCell ref="D56:D57"/>
+    <mergeCell ref="E56:E57"/>
+    <mergeCell ref="C45:C46"/>
+    <mergeCell ref="D45:D46"/>
+    <mergeCell ref="E45:E46"/>
+    <mergeCell ref="C48:C49"/>
+    <mergeCell ref="D48:D49"/>
+    <mergeCell ref="E48:E49"/>
+    <mergeCell ref="C39:C40"/>
+    <mergeCell ref="D39:D40"/>
+    <mergeCell ref="E39:E40"/>
+    <mergeCell ref="C42:C43"/>
+    <mergeCell ref="D42:D43"/>
+    <mergeCell ref="E42:E43"/>
+    <mergeCell ref="F31:G31"/>
+    <mergeCell ref="C33:C34"/>
+    <mergeCell ref="D33:D34"/>
+    <mergeCell ref="E33:E34"/>
+    <mergeCell ref="C36:C37"/>
+    <mergeCell ref="D36:D37"/>
+    <mergeCell ref="E36:E37"/>
+    <mergeCell ref="C25:C26"/>
+    <mergeCell ref="D25:D26"/>
+    <mergeCell ref="E25:E26"/>
+    <mergeCell ref="C28:C29"/>
+    <mergeCell ref="D28:D29"/>
+    <mergeCell ref="E28:E29"/>
+    <mergeCell ref="C19:C20"/>
+    <mergeCell ref="D19:D20"/>
+    <mergeCell ref="E19:E20"/>
+    <mergeCell ref="C22:C23"/>
+    <mergeCell ref="D22:D23"/>
+    <mergeCell ref="E22:E23"/>
+    <mergeCell ref="C2:G4"/>
+    <mergeCell ref="F11:G11"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="D13:D14"/>
+    <mergeCell ref="E13:E14"/>
+    <mergeCell ref="C16:C17"/>
+    <mergeCell ref="D16:D17"/>
+    <mergeCell ref="E16:E17"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="58" orientation="portrait" r:id="rId1"/>

</xml_diff>